<commit_message>
new stock_data and git.txt
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$43</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="52">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,10 +128,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>股票名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -144,67 +140,95 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>第三周周一会跌，主力貌似已经出了大部分货，下周下跌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三周</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.18星期五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.21星期一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多弗多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多弗多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.22星期二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">第三周 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三周</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天赐材料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.23星期三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.23星期三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.24星期四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.24星期四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赣锋锂业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016.3.25星期五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>第三周周一大涨，因为一直在拉高，估计主力建仓完成，成本在55左右，那么下周估计在66左右出货</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第三周周一会跌，主力貌似已经出了大部分货，下周下跌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三周</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.18星期五</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.21星期一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多弗多</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多弗多</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.22星期二</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">第三周 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三周</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>天赐材料</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.23星期三</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.23星期三</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.24星期四</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016.3.24星期四</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赣锋锂业</t>
+    <t>第三周预测总体正确，第四周还会接着涨，因为业绩暴涨，还有高转送，估计除权后还会有一波上升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四周会涨，因为锂电池行业的带动，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三周预测的非常准确，第四周预计跌多涨少了，因为主力的筹码应该不多了，第四周会吸货</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四周会涨，因为锂电池行业的带动，涨幅看到90元，并且主力的筹码应该比较多，建议看情况买入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三周整体预测准确，第四周看涨到155元，因为主力筹码也比较多了，下周涨多跌少，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注(涨red跌black)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -212,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,19 +252,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -266,7 +303,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,20 +619,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="9" width="15.625" style="1"/>
-    <col min="10" max="10" width="23" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="1"/>
+    <col min="3" max="3" width="11.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="50.375" style="1" customWidth="1"/>
     <col min="11" max="16384" width="15.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -591,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -612,10 +669,10 @@
         <v>24</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -645,7 +702,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -675,7 +732,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -705,7 +762,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -735,7 +792,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -765,7 +822,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -795,7 +852,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -825,7 +882,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -855,7 +912,7 @@
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -885,7 +942,7 @@
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -915,7 +972,7 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -945,7 +1002,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -975,7 +1032,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1005,7 +1062,7 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1035,7 +1092,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1065,12 +1122,12 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
@@ -1093,16 +1150,16 @@
       <c r="I17" s="2">
         <v>2.85</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>15</v>
@@ -1125,19 +1182,19 @@
       <c r="I18" s="2">
         <v>4.18</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J18" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D19" s="2">
         <v>-1533</v>
@@ -1157,16 +1214,16 @@
       <c r="I19" s="2">
         <v>2.64</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
@@ -1189,19 +1246,19 @@
       <c r="I20" s="2">
         <v>-1.55</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J20" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D21" s="2">
         <v>168</v>
@@ -1223,15 +1280,15 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2">
         <v>-1192</v>
@@ -1253,12 +1310,12 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
@@ -1283,12 +1340,12 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>10</v>
@@ -1313,12 +1370,12 @@
       </c>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1343,12 +1400,12 @@
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1373,12 +1430,12 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>14</v>
@@ -1403,12 +1460,12 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>14</v>
@@ -1433,15 +1490,15 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2">
         <v>2152</v>
@@ -1463,12 +1520,12 @@
       </c>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>7</v>
@@ -1492,12 +1549,12 @@
         <v>-0.82</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>10</v>
@@ -1521,15 +1578,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" s="1">
         <v>-3709</v>
@@ -1550,12 +1607,12 @@
         <v>-5.04</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1579,12 +1636,12 @@
         <v>-2.76</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>10</v>
@@ -1608,12 +1665,12 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
@@ -1637,15 +1694,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1">
         <v>696</v>
@@ -1666,12 +1723,12 @@
         <v>-0.49</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>5</v>
@@ -1695,15 +1752,15 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D38" s="1">
         <v>829</v>
@@ -1724,8 +1781,168 @@
         <v>2.42</v>
       </c>
     </row>
+    <row r="39" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1">
+        <v>-9691</v>
+      </c>
+      <c r="E39" s="1">
+        <v>69.88</v>
+      </c>
+      <c r="F39" s="1">
+        <v>855</v>
+      </c>
+      <c r="G39" s="1">
+        <v>69.48</v>
+      </c>
+      <c r="H39" s="1">
+        <v>594</v>
+      </c>
+      <c r="I39" s="1">
+        <v>-2.4</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="1">
+        <v>-2730</v>
+      </c>
+      <c r="E40" s="1">
+        <v>45.7</v>
+      </c>
+      <c r="F40" s="1">
+        <v>450</v>
+      </c>
+      <c r="G40" s="1">
+        <v>45.88</v>
+      </c>
+      <c r="H40" s="1">
+        <v>206</v>
+      </c>
+      <c r="I40" s="1">
+        <v>-1.85</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3411</v>
+      </c>
+      <c r="E41" s="1">
+        <v>244.98</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-920</v>
+      </c>
+      <c r="G41" s="1">
+        <v>245.97</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-2262</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="1">
+        <v>-467</v>
+      </c>
+      <c r="E42" s="1">
+        <v>84</v>
+      </c>
+      <c r="F42" s="1">
+        <v>500</v>
+      </c>
+      <c r="G42" s="1">
+        <v>80.319999999999993</v>
+      </c>
+      <c r="H42" s="1">
+        <v>401</v>
+      </c>
+      <c r="I42" s="1">
+        <v>2.94</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="1">
+        <v>-5320</v>
+      </c>
+      <c r="E43" s="1">
+        <v>143.01</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-44</v>
+      </c>
+      <c r="G43" s="1">
+        <v>141</v>
+      </c>
+      <c r="H43" s="1">
+        <v>64</v>
+      </c>
+      <c r="I43" s="1">
+        <v>-2.0499999999999998</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I37"/>
+  <autoFilter ref="A1:I43"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>

</xml_diff>